<commit_message>
Lots of working on skills and XML to streamline
but y tho
</commit_message>
<xml_diff>
--- a/towers/Towers.xlsx
+++ b/towers/Towers.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m3\Documents\GitHub\TowerDefense\towers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spec\Documents\GitHub\TowerDefense\towers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1457C242-C725-43C9-A59F-80B2E15AC768}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF3D81C-805D-4623-ACAF-1A6A4DAB8C90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23220" windowHeight="9495" xr2:uid="{77B776D3-CB80-430E-BB3F-2CE5DE630DB2}"/>
+    <workbookView xWindow="-28920" yWindow="-9810" windowWidth="29040" windowHeight="15840" xr2:uid="{77B776D3-CB80-430E-BB3F-2CE5DE630DB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -35,11 +41,14 @@
   <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="TowersList2" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\m3\Documents\GitHub\TowerDefense\towers\TowersList.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
+  <connection id="4" xr16:uid="{A691AC1E-105E-4818-9B56-80960F8968BC}" name="TowersList3" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\spec\Documents\GitHub\TowerDefense\towers\TowersList.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="171">
   <si>
     <t>Rogue</t>
   </si>
@@ -290,9 +299,6 @@
     <t>earth</t>
   </si>
   <si>
-    <t>Skilled with poisons.  28% slow + 20 dps for 2 seconds.</t>
-  </si>
-  <si>
     <t>Makes a big, poisonous splash when he attacks.  Slows 18% and 5 dmg for 2 seconds.</t>
   </si>
   <si>
@@ -416,9 +422,6 @@
     <t>5 people??  This is madness!  This is an outrage!</t>
   </si>
   <si>
-    <t>Requires a ransom of -1 mIlLiOn DoLlArS- mwuhahaha!</t>
-  </si>
-  <si>
     <t>DeathRay</t>
   </si>
   <si>
@@ -471,6 +474,93 @@
   </si>
   <si>
     <t>Chains 4 additional enemies.</t>
+  </si>
+  <si>
+    <t>Requires a ransom of 1 million dollars.  Thinks that's a lot.</t>
+  </si>
+  <si>
+    <t>skillOne</t>
+  </si>
+  <si>
+    <t>skillTwo</t>
+  </si>
+  <si>
+    <t>skillThree</t>
+  </si>
+  <si>
+    <t>skillFour</t>
+  </si>
+  <si>
+    <t>slow,.25,2</t>
+  </si>
+  <si>
+    <t>hit,poison,.15,3,2</t>
+  </si>
+  <si>
+    <t>hit,poison,.2,5,5</t>
+  </si>
+  <si>
+    <t>hit,poison,.15,5,5</t>
+  </si>
+  <si>
+    <t>hit,brittle,1,3</t>
+  </si>
+  <si>
+    <t>hit,brittle,2,3</t>
+  </si>
+  <si>
+    <t>hit,poison,.20,10,2</t>
+  </si>
+  <si>
+    <t>hit,poison,.18,5,2</t>
+  </si>
+  <si>
+    <t>hit,penitence,.1,2</t>
+  </si>
+  <si>
+    <t>hit,penitence,.15,2</t>
+  </si>
+  <si>
+    <t>hit,burn,5,3</t>
+  </si>
+  <si>
+    <t>hit,burn,15,3</t>
+  </si>
+  <si>
+    <t>hit,slow,.25,2</t>
+  </si>
+  <si>
+    <t>hit,slow,.18,2</t>
+  </si>
+  <si>
+    <t>hit,slow,.28,.5</t>
+  </si>
+  <si>
+    <t>hit,slow,.34,.5</t>
+  </si>
+  <si>
+    <t>hit,slow,.28,3</t>
+  </si>
+  <si>
+    <t>hit,brittle,1,2</t>
+  </si>
+  <si>
+    <t>Skilled with poisons.  28% slow + 20 dps for 5 seconds.</t>
+  </si>
+  <si>
+    <t>hit,poison,.28,20,5</t>
+  </si>
+  <si>
+    <t>hit,chain,3,6,.1,75,fire</t>
+  </si>
+  <si>
+    <t>hit,chain,4,6,.1,75,fire</t>
+  </si>
+  <si>
+    <t>time,atkSpdBuff,.10,2,4,2</t>
+  </si>
+  <si>
+    <t>time,dmgBuff,.12,2,4,2</t>
   </si>
 </sst>
 </file>
@@ -579,7 +669,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -600,21 +690,12 @@
     <xf numFmtId="49" fontId="2" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -696,6 +777,16 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -711,7 +802,7 @@
 
 <file path=xl/xmlMaps.xml><?xml version="1.0" encoding="utf-8"?>
 <MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="">
-  <Schema ID="Schema3">
+  <Schema ID="Schema2">
     <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
       <xsd:element nillable="true" name="Root">
         <xsd:complexType>
@@ -735,6 +826,10 @@
                   <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="upgradeOne" form="unqualified"/>
                   <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="upgradeTwo" form="unqualified"/>
                   <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="upgradeThree" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="skillOne" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="skillTwo" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="skillThree" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="skillFour" form="unqualified"/>
                   <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="targeting" form="unqualified"/>
                 </xsd:all>
               </xsd:complexType>
@@ -744,80 +839,92 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Map ID="3" Name="Root_Map" RootElement="Root" SchemaID="Schema3" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="3" DataBindingLoadMode="1"/>
+  <Map ID="4" Name="TowerList" RootElement="Root" SchemaID="Schema2" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="4" DataBindingLoadMode="1"/>
   </Map>
 </MapInfo>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C71BA424-C6F6-4A20-B1B0-375AB36E248B}" name="Table1" displayName="Table1" ref="A1:W51" tableType="xml" totalsRowShown="0" headerRowDxfId="10" connectionId="3">
-  <autoFilter ref="A1:W51" xr:uid="{7E13DCAC-A1A1-4793-A40C-C0AAEFCA7A3B}"/>
-  <tableColumns count="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C71BA424-C6F6-4A20-B1B0-375AB36E248B}" name="Table1" displayName="Table1" ref="A1:AA51" tableType="xml" totalsRowShown="0" headerRowDxfId="9" connectionId="4">
+  <autoFilter ref="A1:AA51" xr:uid="{7E13DCAC-A1A1-4793-A40C-C0AAEFCA7A3B}"/>
+  <tableColumns count="27">
     <tableColumn id="2" xr3:uid="{BD04A9ED-09E4-4C2F-9A1E-376D27897506}" uniqueName="Name" name="Name">
-      <xmlColumnPr mapId="3" xpath="/Root/Row/Name" xmlDataType="string"/>
+      <xmlColumnPr mapId="4" xpath="/Root/Row/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{DBB8675E-7724-4CE7-AC9D-3B5B328DB5AC}" uniqueName="AoE" name="maxHits" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{DBB8675E-7724-4CE7-AC9D-3B5B328DB5AC}" uniqueName="AoE" name="maxHits" dataDxfId="8"/>
     <tableColumn id="3" xr3:uid="{CB4E03FE-21CD-4530-A347-9FF12F372BD1}" uniqueName="AoE" name="AoE">
-      <xmlColumnPr mapId="3" xpath="/Root/Row/AoE" xmlDataType="integer"/>
+      <xmlColumnPr mapId="4" xpath="/Root/Row/AoE" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{34A04DB4-B101-4D53-AA48-F1BAEB4D37E1}" uniqueName="Range" name="Range">
-      <xmlColumnPr mapId="3" xpath="/Root/Row/Range" xmlDataType="integer"/>
+      <xmlColumnPr mapId="4" xpath="/Root/Row/Range" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{B9C30279-F32E-41E3-B3B1-374F41B7EA21}" uniqueName="of_Targets" name="# of Targets">
-      <xmlColumnPr mapId="3" xpath="/Root/Row/of_Targets" xmlDataType="integer"/>
+      <xmlColumnPr mapId="4" xpath="/Root/Row/of_Targets" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C158085E-F6FA-4A44-B100-6EA300E835B5}" uniqueName="Dmg" name="Dmg" dataDxfId="8">
-      <xmlColumnPr mapId="3" xpath="/Root/Row/Dmg" xmlDataType="integer"/>
+    <tableColumn id="6" xr3:uid="{C158085E-F6FA-4A44-B100-6EA300E835B5}" uniqueName="Dmg" name="Dmg" dataDxfId="7">
+      <xmlColumnPr mapId="4" xpath="/Root/Row/Dmg" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{1207337A-E6BF-4DD9-AB32-5D838856DA34}" uniqueName="Atk_Speed" name="Atk Speed" dataDxfId="7">
-      <xmlColumnPr mapId="3" xpath="/Root/Row/Atk_Speed" xmlDataType="integer"/>
+    <tableColumn id="7" xr3:uid="{1207337A-E6BF-4DD9-AB32-5D838856DA34}" uniqueName="Atk_Speed" name="Atk Speed" dataDxfId="6">
+      <xmlColumnPr mapId="4" xpath="/Root/Row/Atk_Speed" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{EB7D4130-A460-4772-B3AD-98C34232A5B7}" uniqueName="Cost" name="Cost" dataDxfId="6">
-      <xmlColumnPr mapId="3" xpath="/Root/Row/Cost" xmlDataType="integer"/>
+    <tableColumn id="8" xr3:uid="{EB7D4130-A460-4772-B3AD-98C34232A5B7}" uniqueName="Cost" name="Cost" dataDxfId="5">
+      <xmlColumnPr mapId="4" xpath="/Root/Row/Cost" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{CDADC387-2692-4651-A063-1A76B0415D0D}" uniqueName="bulletFrame" name="Total Cost" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{CDADC387-2692-4651-A063-1A76B0415D0D}" uniqueName="bulletFrame" name="Total Cost" dataDxfId="4"/>
     <tableColumn id="10" xr3:uid="{960B1B92-4605-4C0A-9012-0A2C4A9B7786}" uniqueName="Type" name="Type">
-      <xmlColumnPr mapId="3" xpath="/Root/Row/Type" xmlDataType="string"/>
+      <xmlColumnPr mapId="4" xpath="/Root/Row/Type" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{F406916D-AC1F-4D7C-91E2-3C08BF8F9390}" uniqueName="towerFrame" name="Min DPS" dataDxfId="4">
+    <tableColumn id="12" xr3:uid="{F406916D-AC1F-4D7C-91E2-3C08BF8F9390}" uniqueName="towerFrame" name="Min DPS" dataDxfId="3">
       <calculatedColumnFormula>SUM(F2*(24/G2))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{3165D01F-EC46-48DE-8129-008D610D5BB8}" uniqueName="fireSoundString" name="Max DPS" dataDxfId="3">
+    <tableColumn id="13" xr3:uid="{3165D01F-EC46-48DE-8129-008D610D5BB8}" uniqueName="fireSoundString" name="Max DPS" dataDxfId="2">
       <calculatedColumnFormula>SUM(F2*(24/G2))*E2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{79A19EDE-9D24-4FD1-BD5F-613A5DE27DA6}" uniqueName="tDescription" name="Gold per Min DPS" dataDxfId="2">
+    <tableColumn id="14" xr3:uid="{79A19EDE-9D24-4FD1-BD5F-613A5DE27DA6}" uniqueName="tDescription" name="Gold per Min DPS" dataDxfId="1">
       <calculatedColumnFormula>SUM(I2/K2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{A26755EC-DC65-4209-BFD6-9F0002BCD397}" uniqueName="upgradeOne" name="G/M.DPS" dataDxfId="1">
+    <tableColumn id="15" xr3:uid="{A26755EC-DC65-4209-BFD6-9F0002BCD397}" uniqueName="upgradeOne" name="G/M.DPS" dataDxfId="0">
       <calculatedColumnFormula>SUM(I2/L2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="16" xr3:uid="{C3F60BD1-F34D-480E-93CD-521D41E09EB5}" uniqueName="bulletFrame" name="bulletFrame">
-      <xmlColumnPr mapId="3" xpath="/Root/Row/bulletFrame" xmlDataType="integer"/>
+      <xmlColumnPr mapId="4" xpath="/Root/Row/bulletFrame" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="17" xr3:uid="{D6FE27F0-9BA9-4042-A2FB-7EB813A3CD4E}" uniqueName="bulletSpeed" name="bulletSpeed">
-      <xmlColumnPr mapId="3" xpath="/Root/Row/bulletSpeed" xmlDataType="integer"/>
+      <xmlColumnPr mapId="4" xpath="/Root/Row/bulletSpeed" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="18" xr3:uid="{3D7ECFAE-69C7-4D3F-B8EF-DE3456EED59C}" uniqueName="towerFrame" name="towerFrame">
-      <xmlColumnPr mapId="3" xpath="/Root/Row/towerFrame" xmlDataType="integer"/>
+      <xmlColumnPr mapId="4" xpath="/Root/Row/towerFrame" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="19" xr3:uid="{483C72D6-B33C-452D-BE8F-E524D370C58C}" uniqueName="fireSoundString" name="fireSoundString">
-      <xmlColumnPr mapId="3" xpath="/Root/Row/fireSoundString" xmlDataType="string"/>
+      <xmlColumnPr mapId="4" xpath="/Root/Row/fireSoundString" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="20" xr3:uid="{3624DC5F-C196-4453-A4C0-CB17DCE76751}" uniqueName="tDescription" name="tDescription">
-      <xmlColumnPr mapId="3" xpath="/Root/Row/tDescription" xmlDataType="string"/>
+      <xmlColumnPr mapId="4" xpath="/Root/Row/tDescription" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="11" xr3:uid="{1B12F4CC-722E-4BFB-9EA8-7BC8CB93A247}" uniqueName="upgradeOne" name="upgradeOne">
-      <xmlColumnPr mapId="3" xpath="/Root/Row/upgradeOne" xmlDataType="string"/>
+      <xmlColumnPr mapId="4" xpath="/Root/Row/upgradeOne" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="21" xr3:uid="{95D68C7E-6AEC-4AC2-B5B4-1E2C3EDE848C}" uniqueName="upgradeTwo" name="upgradeTwo">
-      <xmlColumnPr mapId="3" xpath="/Root/Row/upgradeTwo" xmlDataType="string"/>
+      <xmlColumnPr mapId="4" xpath="/Root/Row/upgradeTwo" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="22" xr3:uid="{9DBC30FB-5F26-4DBD-945C-43FD0F36F2A8}" uniqueName="upgradeThree" name="upgradeThree">
-      <xmlColumnPr mapId="3" xpath="/Root/Row/upgradeThree" xmlDataType="string"/>
+      <xmlColumnPr mapId="4" xpath="/Root/Row/upgradeThree" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="23" xr3:uid="{E256A08A-04FD-4A56-951F-6AF7E250751B}" uniqueName="targeting" name="targeting">
-      <xmlColumnPr mapId="3" xpath="/Root/Row/targeting" xmlDataType="string"/>
+      <xmlColumnPr mapId="4" xpath="/Root/Row/targeting" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="24" xr3:uid="{14F20794-1BBA-4281-97D1-1B39B6A60726}" uniqueName="skillOne" name="skillOne">
+      <xmlColumnPr mapId="4" xpath="/Root/Row/skillOne" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="25" xr3:uid="{FAF0774D-00DD-4CE6-B71C-583ACCEF47B3}" uniqueName="skillTwo" name="skillTwo">
+      <xmlColumnPr mapId="4" xpath="/Root/Row/skillTwo" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="26" xr3:uid="{7333556A-ED46-4116-BAE2-72C5F5C79C7D}" uniqueName="skillThree" name="skillThree">
+      <xmlColumnPr mapId="4" xpath="/Root/Row/skillThree" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="27" xr3:uid="{3E110F20-4559-4331-BCD4-B34F6EF3F7B2}" uniqueName="skillFour" name="skillFour">
+      <xmlColumnPr mapId="4" xpath="/Root/Row/skillFour" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1122,12 +1229,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A7CA67B-E2EB-42AB-840C-E4EC35DF9DA8}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:W51"/>
+  <dimension ref="A1:AA51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
       <selection activeCell="A19" sqref="A19"/>
-      <selection pane="topRight" activeCell="Q50" sqref="Q50"/>
+      <selection pane="topRight" activeCell="X19" sqref="X19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1136,24 +1243,29 @@
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="128" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="107" customWidth="1"/>
+    <col min="20" max="20" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>25</v>
       </c>
@@ -1212,19 +1324,31 @@
         <v>36</v>
       </c>
       <c r="T1" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="U1" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="V1" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="W1" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="W1" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y1" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z1" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="AA1" s="9" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>37</v>
       </c>
@@ -1286,7 +1410,7 @@
         <v>54</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U2" s="6" t="s">
         <v>3</v>
@@ -1295,8 +1419,12 @@
         <v>0</v>
       </c>
       <c r="W2" s="6"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6"/>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
@@ -1355,7 +1483,7 @@
         <v>56</v>
       </c>
       <c r="S3" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="T3" s="6" t="s">
         <v>4</v>
@@ -1365,8 +1493,14 @@
       </c>
       <c r="V3" s="6"/>
       <c r="W3" s="6"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X3" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="6"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>4</v>
       </c>
@@ -1425,14 +1559,20 @@
         <v>56</v>
       </c>
       <c r="S4" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="T4" s="6"/>
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
       <c r="W4" s="6"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X4" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+      <c r="AA4" s="6"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
@@ -1497,8 +1637,14 @@
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
       <c r="W5" s="6"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X5" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+      <c r="AA5" s="6"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>2</v>
       </c>
@@ -1567,8 +1713,14 @@
       </c>
       <c r="V6" s="6"/>
       <c r="W6" s="6"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X6" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
+      <c r="AA6" s="6"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>5</v>
       </c>
@@ -1633,8 +1785,14 @@
       <c r="U7" s="6"/>
       <c r="V7" s="6"/>
       <c r="W7" s="6"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X7" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="6"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
@@ -1699,8 +1857,14 @@
       <c r="U8" s="6"/>
       <c r="V8" s="6"/>
       <c r="W8" s="6"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X8" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>3</v>
       </c>
@@ -1759,7 +1923,7 @@
         <v>52</v>
       </c>
       <c r="S9" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="T9" s="6" t="s">
         <v>7</v>
@@ -1769,8 +1933,14 @@
       </c>
       <c r="V9" s="6"/>
       <c r="W9" s="6"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X9" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y9" s="6"/>
+      <c r="Z9" s="6"/>
+      <c r="AA9" s="6"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>7</v>
       </c>
@@ -1829,14 +1999,20 @@
         <v>52</v>
       </c>
       <c r="S10" s="6" t="s">
-        <v>83</v>
+        <v>165</v>
       </c>
       <c r="T10" s="6"/>
       <c r="U10" s="6"/>
       <c r="V10" s="6"/>
       <c r="W10" s="6"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X10" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
+      <c r="AA10" s="6"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
@@ -1897,14 +2073,20 @@
         <v>67</v>
       </c>
       <c r="S11" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="T11" s="6"/>
       <c r="U11" s="6"/>
       <c r="V11" s="6"/>
       <c r="W11" s="6"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X11" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="6"/>
+      <c r="AA11" s="6"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>68</v>
       </c>
@@ -1975,8 +2157,12 @@
         <v>38</v>
       </c>
       <c r="W12" s="6"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X12" s="6"/>
+      <c r="Y12" s="6"/>
+      <c r="Z12" s="6"/>
+      <c r="AA12" s="6"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>38</v>
       </c>
@@ -2041,12 +2227,16 @@
         <v>39</v>
       </c>
       <c r="U13" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="V13" s="6"/>
       <c r="W13" s="6"/>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X13" s="6"/>
+      <c r="Y13" s="6"/>
+      <c r="Z13" s="6"/>
+      <c r="AA13" s="6"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>39</v>
       </c>
@@ -2111,8 +2301,12 @@
       <c r="U14" s="6"/>
       <c r="V14" s="6"/>
       <c r="W14" s="6"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X14" s="6"/>
+      <c r="Y14" s="6"/>
+      <c r="Z14" s="6"/>
+      <c r="AA14" s="6"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>81</v>
       </c>
@@ -2177,8 +2371,12 @@
       <c r="U15" s="6"/>
       <c r="V15" s="6"/>
       <c r="W15" s="6"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X15" s="6"/>
+      <c r="Y15" s="6"/>
+      <c r="Z15" s="6"/>
+      <c r="AA15" s="6"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>41</v>
       </c>
@@ -2240,13 +2438,19 @@
         <v>61</v>
       </c>
       <c r="T16" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="U16" s="6"/>
       <c r="V16" s="6"/>
       <c r="W16" s="6"/>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X16" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y16" s="6"/>
+      <c r="Z16" s="6"/>
+      <c r="AA16" s="6"/>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>40</v>
       </c>
@@ -2305,14 +2509,20 @@
         <v>50</v>
       </c>
       <c r="S17" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="T17" s="6"/>
       <c r="U17" s="6"/>
       <c r="V17" s="6"/>
       <c r="W17" s="6"/>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X17" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="Y17" s="6"/>
+      <c r="Z17" s="6"/>
+      <c r="AA17" s="6"/>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>42</v>
       </c>
@@ -2377,8 +2587,12 @@
       <c r="U18" s="6"/>
       <c r="V18" s="6"/>
       <c r="W18" s="6"/>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X18" s="6"/>
+      <c r="Y18" s="6"/>
+      <c r="Z18" s="6"/>
+      <c r="AA18" s="6"/>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>43</v>
       </c>
@@ -2437,14 +2651,20 @@
         <v>50</v>
       </c>
       <c r="S19" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="T19" s="6"/>
       <c r="U19" s="6"/>
       <c r="V19" s="6"/>
       <c r="W19" s="6"/>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X19" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="Y19" s="6"/>
+      <c r="Z19" s="6"/>
+      <c r="AA19" s="6"/>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>44</v>
       </c>
@@ -2507,8 +2727,12 @@
       <c r="U20" s="6"/>
       <c r="V20" s="6"/>
       <c r="W20" s="6"/>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X20" s="6"/>
+      <c r="Y20" s="6"/>
+      <c r="Z20" s="6"/>
+      <c r="AA20" s="6"/>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>45</v>
       </c>
@@ -2571,8 +2795,12 @@
       <c r="U21" s="6"/>
       <c r="V21" s="6"/>
       <c r="W21" s="6"/>
-    </row>
-    <row r="22" spans="1:23" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="X21" s="6"/>
+      <c r="Y21" s="6"/>
+      <c r="Z21" s="6"/>
+      <c r="AA21" s="6"/>
+    </row>
+    <row r="22" spans="1:27" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>69</v>
       </c>
@@ -2634,17 +2862,21 @@
         <v>63</v>
       </c>
       <c r="T22" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="U22" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="U22" s="6" t="s">
+      <c r="V22" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="V22" s="6" t="s">
-        <v>113</v>
-      </c>
       <c r="W22" s="6"/>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X22" s="6"/>
+      <c r="Y22" s="6"/>
+      <c r="Z22" s="6"/>
+      <c r="AA22" s="6"/>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>46</v>
       </c>
@@ -2705,20 +2937,24 @@
         <v>67</v>
       </c>
       <c r="S23" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="T23" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="U23" s="6"/>
       <c r="V23" s="6"/>
       <c r="W23" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="X23" s="6"/>
+      <c r="Y23" s="6"/>
+      <c r="Z23" s="6"/>
+      <c r="AA23" s="6"/>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B24" s="7">
         <v>5</v>
@@ -2777,18 +3013,22 @@
         <v>67</v>
       </c>
       <c r="S24" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="T24" s="6"/>
       <c r="U24" s="6"/>
       <c r="V24" s="6"/>
       <c r="W24" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="X24" s="6"/>
+      <c r="Y24" s="6"/>
+      <c r="Z24" s="6"/>
+      <c r="AA24" s="6"/>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B25" s="6"/>
       <c r="F25" s="1"/>
@@ -2826,10 +3066,14 @@
       <c r="U25" s="6"/>
       <c r="V25" s="6"/>
       <c r="W25" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="X25" s="6"/>
+      <c r="Y25" s="6"/>
+      <c r="Z25" s="6"/>
+      <c r="AA25" s="6"/>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>71</v>
       </c>
@@ -2891,15 +3135,19 @@
         <v>65</v>
       </c>
       <c r="T26" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="U26" s="6"/>
       <c r="V26" s="6"/>
       <c r="W26" s="6"/>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X26" s="6"/>
+      <c r="Y26" s="6"/>
+      <c r="Z26" s="6"/>
+      <c r="AA26" s="6"/>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27">
@@ -2956,16 +3204,20 @@
         <v>64</v>
       </c>
       <c r="S27" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T27" s="6"/>
       <c r="U27" s="6"/>
       <c r="V27" s="6"/>
       <c r="W27" s="6"/>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X27" s="6"/>
+      <c r="Y27" s="6"/>
+      <c r="Z27" s="6"/>
+      <c r="AA27" s="6"/>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B28" s="6"/>
       <c r="F28" s="1"/>
@@ -3000,8 +3252,12 @@
       <c r="U28" s="6"/>
       <c r="V28" s="6"/>
       <c r="W28" s="6"/>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X28" s="6"/>
+      <c r="Y28" s="6"/>
+      <c r="Z28" s="6"/>
+      <c r="AA28" s="6"/>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>47</v>
       </c>
@@ -3065,15 +3321,21 @@
         <v>58</v>
       </c>
       <c r="T29" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="U29" s="6"/>
       <c r="V29" s="6"/>
       <c r="W29" s="6"/>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X29" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="Y29" s="6"/>
+      <c r="Z29" s="6"/>
+      <c r="AA29" s="6"/>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B30" s="7">
         <v>3</v>
@@ -3132,16 +3394,22 @@
         <v>67</v>
       </c>
       <c r="S30" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="T30" s="6"/>
       <c r="U30" s="6"/>
       <c r="V30" s="6"/>
       <c r="W30" s="6"/>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X30" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y30" s="6"/>
+      <c r="Z30" s="6"/>
+      <c r="AA30" s="6"/>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B31" s="6"/>
       <c r="F31" s="1"/>
@@ -3176,8 +3444,12 @@
       <c r="U31" s="6"/>
       <c r="V31" s="6"/>
       <c r="W31" s="6"/>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X31" s="6"/>
+      <c r="Y31" s="6"/>
+      <c r="Z31" s="6"/>
+      <c r="AA31" s="6"/>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>70</v>
       </c>
@@ -3238,22 +3510,28 @@
         <v>67</v>
       </c>
       <c r="S32" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="T32" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="U32" s="6" t="s">
         <v>80</v>
       </c>
       <c r="V32" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="W32" s="6"/>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X32" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="Y32" s="6"/>
+      <c r="Z32" s="6"/>
+      <c r="AA32" s="6"/>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B33" s="7">
         <v>3</v>
@@ -3312,18 +3590,24 @@
         <v>67</v>
       </c>
       <c r="S33" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="T33" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="U33" s="6"/>
       <c r="V33" s="6"/>
       <c r="W33" s="6"/>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X33" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="Y33" s="6"/>
+      <c r="Z33" s="6"/>
+      <c r="AA33" s="6"/>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B34" s="7">
         <v>3</v>
@@ -3382,14 +3666,20 @@
         <v>67</v>
       </c>
       <c r="S34" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="T34" s="6"/>
       <c r="U34" s="6"/>
       <c r="V34" s="6"/>
       <c r="W34" s="6"/>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X34" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="Y34" s="6"/>
+      <c r="Z34" s="6"/>
+      <c r="AA34" s="6"/>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
         <v>80</v>
       </c>
@@ -3448,18 +3738,26 @@
         <v>67</v>
       </c>
       <c r="S35" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="T35" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="U35" s="6"/>
       <c r="V35" s="6"/>
       <c r="W35" s="6"/>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X35" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="Y35" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="Z35" s="6"/>
+      <c r="AA35" s="6"/>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36">
@@ -3516,14 +3814,22 @@
         <v>67</v>
       </c>
       <c r="S36" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="T36" s="6"/>
       <c r="U36" s="6"/>
       <c r="V36" s="6"/>
       <c r="W36" s="6"/>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X36" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="Y36" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="Z36" s="6"/>
+      <c r="AA36" s="6"/>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
         <v>48</v>
       </c>
@@ -3584,22 +3890,28 @@
         <v>67</v>
       </c>
       <c r="S37" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T37" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U37" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="V37" s="6"/>
       <c r="W37" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="X37" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y37" s="6"/>
+      <c r="Z37" s="6"/>
+      <c r="AA37" s="6"/>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B38" s="7">
         <v>4</v>
@@ -3658,18 +3970,24 @@
         <v>67</v>
       </c>
       <c r="S38" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="T38" s="6"/>
       <c r="U38" s="6"/>
       <c r="V38" s="6"/>
       <c r="W38" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="X38" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y38" s="6"/>
+      <c r="Z38" s="6"/>
+      <c r="AA38" s="6"/>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B39" s="7">
         <v>2</v>
@@ -3728,14 +4046,20 @@
         <v>67</v>
       </c>
       <c r="S39" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="T39" s="6"/>
       <c r="U39" s="6"/>
       <c r="V39" s="6"/>
       <c r="W39" s="6"/>
-    </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X39" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="Y39" s="6"/>
+      <c r="Z39" s="6"/>
+      <c r="AA39" s="6"/>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
         <v>19</v>
       </c>
@@ -3799,15 +4123,19 @@
         <v>55</v>
       </c>
       <c r="T40" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="U40" s="6" t="s">
         <v>21</v>
       </c>
       <c r="V40" s="6"/>
       <c r="W40" s="6"/>
-    </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X40" s="6"/>
+      <c r="Y40" s="6"/>
+      <c r="Z40" s="6"/>
+      <c r="AA40" s="6"/>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
         <v>49</v>
       </c>
@@ -3871,15 +4199,19 @@
         <v>66</v>
       </c>
       <c r="T41" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="U41" s="6"/>
       <c r="V41" s="6"/>
       <c r="W41" s="6"/>
-    </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X41" s="6"/>
+      <c r="Y41" s="6"/>
+      <c r="Z41" s="6"/>
+      <c r="AA41" s="6"/>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B42" s="7">
         <v>3</v>
@@ -3938,14 +4270,18 @@
         <v>67</v>
       </c>
       <c r="S42" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="T42" s="6"/>
       <c r="U42" s="6"/>
       <c r="V42" s="6"/>
       <c r="W42" s="6"/>
-    </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X42" s="6"/>
+      <c r="Y42" s="6"/>
+      <c r="Z42" s="6"/>
+      <c r="AA42" s="6"/>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
         <v>21</v>
       </c>
@@ -4007,15 +4343,19 @@
         <v>62</v>
       </c>
       <c r="T43" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U43" s="6"/>
       <c r="V43" s="6"/>
       <c r="W43" s="6"/>
-    </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X43" s="6"/>
+      <c r="Y43" s="6"/>
+      <c r="Z43" s="6"/>
+      <c r="AA43" s="6"/>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B44" s="6"/>
       <c r="C44">
@@ -4072,14 +4412,18 @@
         <v>67</v>
       </c>
       <c r="S44" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="T44" s="6"/>
       <c r="U44" s="6"/>
       <c r="V44" s="6"/>
       <c r="W44" s="6"/>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X44" s="6"/>
+      <c r="Y44" s="6"/>
+      <c r="Z44" s="6"/>
+      <c r="AA44" s="6"/>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
         <v>29</v>
       </c>
@@ -4147,11 +4491,15 @@
         <v>20</v>
       </c>
       <c r="V45" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="W45" s="6"/>
-    </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X45" s="6"/>
+      <c r="Y45" s="6"/>
+      <c r="Z45" s="6"/>
+      <c r="AA45" s="6"/>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
         <v>30</v>
       </c>
@@ -4213,15 +4561,19 @@
         <v>57</v>
       </c>
       <c r="T46" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U46" s="6"/>
       <c r="V46" s="6"/>
       <c r="W46" s="6"/>
-    </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X46" s="6"/>
+      <c r="Y46" s="6"/>
+      <c r="Z46" s="6"/>
+      <c r="AA46" s="6"/>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B47" s="6"/>
       <c r="C47">
@@ -4278,14 +4630,18 @@
         <v>67</v>
       </c>
       <c r="S47" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="T47" s="6"/>
       <c r="U47" s="6"/>
       <c r="V47" s="6"/>
       <c r="W47" s="6"/>
-    </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X47" s="6"/>
+      <c r="Y47" s="6"/>
+      <c r="Z47" s="6"/>
+      <c r="AA47" s="6"/>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" s="18" t="s">
         <v>20</v>
       </c>
@@ -4347,15 +4703,19 @@
         <v>60</v>
       </c>
       <c r="T48" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="U48" s="6"/>
       <c r="V48" s="6"/>
       <c r="W48" s="6"/>
-    </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X48" s="6"/>
+      <c r="Y48" s="6"/>
+      <c r="Z48" s="6"/>
+      <c r="AA48" s="6"/>
+    </row>
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A49" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B49" s="6"/>
       <c r="C49">
@@ -4412,15 +4772,20 @@
         <v>67</v>
       </c>
       <c r="S49" s="6" t="s">
-        <v>125</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="T49" s="6"/>
       <c r="U49" s="6"/>
       <c r="V49" s="6"/>
       <c r="W49" s="6"/>
-    </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X49" s="6"/>
+      <c r="Y49" s="6"/>
+      <c r="Z49" s="6"/>
+      <c r="AA49" s="6"/>
+    </row>
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B50" s="7">
         <v>3</v>
@@ -4479,18 +4844,24 @@
         <v>67</v>
       </c>
       <c r="S50" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="T50" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="U50" s="6"/>
       <c r="V50" s="6"/>
       <c r="W50" s="6"/>
-    </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X50" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y50" s="6"/>
+      <c r="Z50" s="6"/>
+      <c r="AA50" s="6"/>
+    </row>
+    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51" s="18" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B51" s="7">
         <v>4</v>
@@ -4542,19 +4913,25 @@
       <c r="P51" s="7">
         <v>20</v>
       </c>
-      <c r="Q51" s="7">
+      <c r="Q51" s="20">
         <v>45</v>
       </c>
       <c r="R51" s="6" t="s">
         <v>67</v>
       </c>
       <c r="S51" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="T51" s="6"/>
       <c r="U51" s="6"/>
       <c r="V51" s="6"/>
       <c r="W51" s="6"/>
+      <c r="X51" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="Y51" s="6"/>
+      <c r="Z51" s="6"/>
+      <c r="AA51" s="6"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="J52:J1048576 I1:I51">
@@ -4570,7 +4947,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q1048576">
-    <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="2"/>
+    <cfRule type="top10" dxfId="10" priority="1" percent="1" rank="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>